<commit_message>
replacing bug report 0.3
replacing bug report 0.3
</commit_message>
<xml_diff>
--- a/The Riflemen/The Riflemen - Bug Report 0.3.xlsx
+++ b/The Riflemen/The Riflemen - Bug Report 0.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bened\OneDrive\Desktop\Game Testing\The Riflemen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0042F5C5-59B7-49A2-A8FE-8B726A189A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659FDB3B-C8B1-4260-864A-5FB9A9DA4041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="124">
   <si>
     <t>Project Details</t>
   </si>
@@ -279,9 +279,6 @@
     <t>the rocket of a bazooka is launched from the end of the weapon</t>
   </si>
   <si>
-    <t>the rocket of a bazooka is lauched from the top of where the weapon begins</t>
-  </si>
-  <si>
     <t>Rifbug 11</t>
   </si>
   <si>
@@ -357,9 +354,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>lehet csak oda megy vissza ahol megmurdeltem</t>
-  </si>
-  <si>
     <t>Rifbug 13</t>
   </si>
   <si>
@@ -367,10 +361,6 @@
   </si>
   <si>
     <t>log into another player's lobby</t>
-  </si>
-  <si>
-    <t>When the guest player in another player's lobby, shoots all ammos and gets Supply Drop Greneada and tries to throw it, the grenada always remains in guest player's hand in its point of view.
-In an enemy's point of view, after guest player shoots all ammos it sees the Bolt Riffle instead of the grenade. When this bug is performed, the guest player cannot harm enemy player.</t>
   </si>
   <si>
     <t>throw Supply Drop Grenade</t>
@@ -402,6 +392,13 @@
   <si>
     <t>Benedek Sándor Seres, benedek.seres@gmail.com
 Lilla Seres, vajdulak.lilla@gmail.com</t>
+  </si>
+  <si>
+    <t>the rocket of a bazooka is launched from the top of where the weapon begins</t>
+  </si>
+  <si>
+    <t>When the guest player in another player's lobby, shoots all ammos and gets Supply Drop Grenade and tries to throw it, the grenade always remains in guest player's hand in its point of view.
+In an enemy's point of view, after guest player shoots all ammos it sees the Bolt Riffle instead of the grenade. When this bug is performed, the guest player cannot harm enemy player.</t>
   </si>
 </sst>
 </file>
@@ -666,6 +663,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="15" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,6 +678,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -706,18 +715,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1191,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,79 +1204,79 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="16" t="s">
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="2:8" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+      <c r="B6" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="32"/>
       <c r="H6" s="33"/>
     </row>
     <row r="7" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="16" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
@@ -1759,10 +1756,10 @@
         <v>70</v>
       </c>
       <c r="C45" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>81</v>
@@ -1771,7 +1768,7 @@
         <v>83</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>24</v>
@@ -1793,7 +1790,7 @@
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -1813,19 +1810,19 @@
         <v>80</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>81</v>
       </c>
       <c r="F49" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G49" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>18</v>
@@ -1836,7 +1833,7 @@
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -1848,7 +1845,7 @@
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -1866,22 +1863,22 @@
     </row>
     <row r="53" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F53" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G53" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>18</v>
@@ -1893,7 +1890,7 @@
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -1904,7 +1901,7 @@
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -1921,35 +1918,33 @@
     </row>
     <row r="57" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="D57" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="E57" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="F57" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G57" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G57" s="4" t="s">
+      <c r="H57" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="58" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="4"/>
-      <c r="C58" s="4" t="s">
-        <v>110</v>
-      </c>
+      <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -1966,25 +1961,25 @@
     </row>
     <row r="60" spans="2:10" ht="165" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>113</v>
-      </c>
       <c r="F60" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
@@ -1992,7 +1987,7 @@
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -2003,7 +1998,7 @@
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -2014,7 +2009,7 @@
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -2025,7 +2020,7 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -2036,7 +2031,7 @@
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>

</xml_diff>